<commit_message>
Testing Author blobs passed Language blobs fix Helper Spliters fix Build passed
</commit_message>
<xml_diff>
--- a/quanlythuvien/data/List_TacGia.xlsx
+++ b/quanlythuvien/data/List_TacGia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\New folder (2)\mini-library-manager\quanlythuvien\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C110D3-9314-420C-B3ED-5B7C6DA8A7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149E3BB3-E3F3-49FC-8715-BB62AA624CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,7 +627,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +656,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -679,7 +685,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -689,26 +695,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,16 +984,17 @@
   <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A58"/>
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="74.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="74.28515625" customWidth="1"/>
     <col min="7" max="7" width="53.42578125" customWidth="1"/>
     <col min="8" max="8" width="26.140625" customWidth="1"/>
     <col min="9" max="9" width="33.140625" customWidth="1"/>
@@ -1005,2368 +1003,1934 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="3" t="str">
+      <c r="E2" s="1" t="str">
         <f>CONCATENATE(SUBSTITUTE(B2," ",""),"",,"@gmail.com")</f>
         <v>HoangNgocQuang@gmail.com</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5" t="str">
+      <c r="G2" t="str">
         <f>CONCATENATE("https://sites.google.com/site/","",SUBSTITUTE(B2," ",""))</f>
         <v>https://sites.google.com/site/HoangNgocQuang</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D14" si="0">CONCATENATE(SUBSTITUTE(B3," ",""),"",,"@gmail.com")</f>
+      <c r="E3" s="1" t="str">
+        <f t="shared" ref="E3:E14" si="0">CONCATENATE(SUBSTITUTE(B3," ",""),"",,"@gmail.com")</f>
         <v>HoangHongQuy@gmail.com</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="5" t="str">
+      <c r="G3" t="str">
         <f t="shared" ref="G3:G14" si="1">CONCATENATE("https://sites.google.com/site/","",SUBSTITUTE(B3," ",""))</f>
         <v>https://sites.google.com/site/HoangHongQuy</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="3" t="str">
+      <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangNgocTru@gmail.com</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="str">
+      <c r="G4" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangNgocTru</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="3" t="str">
+      <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangTheAnh@gmail.com</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5" t="str">
+      <c r="G5" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangTheAnh</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D6" s="3" t="str">
+      <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangDuongAnh@gmail.com</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="5" t="str">
+      <c r="G6" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangDuongAnh</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="3">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="3" t="str">
+      <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangHongThinh@gmail.com</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="5" t="str">
+      <c r="G7" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangHongThinh</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="3">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D8" s="3" t="str">
+      <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangQuocMinh@gmail.com</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="5" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangQuocMinh</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="3">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="3" t="str">
+      <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangTheSon@gmail.com</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="5" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangTheSon</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="3" t="str">
+      <c r="E10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangThanhNguyen@gmail.com</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="5" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangThanhNguyen</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="E11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>HoangAnNam@gmail.com</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="5" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/HoangAnNam</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D12" s="3" t="str">
+      <c r="E12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>TranUyenNhi@gmail.com</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="5" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/TranUyenNhi</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="3">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>TranNhatThuong@gmail.com</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="5" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/TranNhatThuong</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="E14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>TranVietTuyet@gmail.com</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="5" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="1"/>
         <v>https://sites.google.com/site/TranVietTuyet</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="3">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D15" s="3" t="str">
-        <f t="shared" ref="D15:D29" si="2">CONCATENATE(SUBSTITUTE(B15," ",""),"",,"@gmail.com")</f>
+      <c r="E15" s="1" t="str">
+        <f t="shared" ref="E15:E29" si="2">CONCATENATE(SUBSTITUTE(B15," ",""),"",,"@gmail.com")</f>
         <v>TranViAn@gmail.com</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="5" t="str">
+      <c r="G15" t="str">
         <f t="shared" ref="G15:G29" si="3">CONCATENATE("https://sites.google.com/site/","",SUBSTITUTE(B15," ",""))</f>
         <v>https://sites.google.com/site/TranViAn</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="3">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D16" s="3" t="str">
+      <c r="E16" s="1" t="str">
         <f t="shared" si="2"/>
         <v>TranBichPhuong@gmail.com</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="5" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/TranBichPhuong</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="3">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="E17" s="1" t="str">
         <f t="shared" si="2"/>
         <v>TranNgocDiem@gmail.com</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="5" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/TranNgocDiem</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="3">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="E18" s="1" t="str">
         <f t="shared" si="2"/>
         <v>TranMinhNgan@gmail.com</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="5" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/TranMinhNgan</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="3">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="E19" s="1" t="str">
         <f t="shared" si="2"/>
         <v>TranThienGiang@gmail.com</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="5" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/TranThienGiang</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="3">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="E20" s="1" t="str">
         <f t="shared" si="2"/>
         <v>TranAiNhi@gmail.com</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="5" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/TranAiNhi</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" t="s">
         <v>60</v>
       </c>
-      <c r="I20" s="9"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="3">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="E21" s="1" t="str">
         <f t="shared" si="2"/>
         <v>TranCamChi@gmail.com</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="5" t="str">
+      <c r="G21" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/TranCamChi</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" t="s">
         <v>72</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="3">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D22" s="3" t="str">
+      <c r="E22" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenQuangThong@gmail.com</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="F22" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="5" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenQuangThong</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" t="s">
         <v>72</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="3">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D23" s="3" t="str">
+      <c r="E23" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenNgocThach@gmail.com</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="5" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenNgocThach</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" t="s">
         <v>72</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="3">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D24" s="3" t="str">
+      <c r="E24" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenThanhThien@gmail.com</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="F24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="5" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenThanhThien</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" t="s">
         <v>72</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="3">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D25" s="3" t="str">
+      <c r="E25" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenTruongAn@gmail.com</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="5" t="str">
+      <c r="G25" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenTruongAn</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" t="s">
         <v>72</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="3">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D26" s="3" t="str">
+      <c r="E26" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenKhaiTam@gmail.com</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="5" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenKhaiTam</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" t="s">
         <v>72</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="3">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D27" s="3" t="str">
+      <c r="E27" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenDuyHung@gmail.com</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" s="5" t="str">
+      <c r="G27" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenDuyHung</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" t="s">
         <v>72</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="3">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="3" t="str">
+      <c r="E28" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenAnhThai@gmail.com</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="F28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G28" s="5" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenAnhThai</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" t="s">
         <v>72</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="3">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="E29" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NguyenGiaThien@gmail.com</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="5" t="str">
+      <c r="G29" t="str">
         <f t="shared" si="3"/>
         <v>https://sites.google.com/site/NguyenGiaThien</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" t="s">
         <v>72</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="3">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" ref="D30:D44" si="4">CONCATENATE(SUBSTITUTE(B30," ",""),"",,"@gmail.com")</f>
+      <c r="E30" s="1" t="str">
+        <f t="shared" ref="E30:E44" si="4">CONCATENATE(SUBSTITUTE(B30," ",""),"",,"@gmail.com")</f>
         <v>NguyenBaoLan@gmail.com</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G30" s="5" t="str">
+      <c r="G30" t="str">
         <f t="shared" ref="G30:G43" si="5">CONCATENATE("https://sites.google.com/site/","",SUBSTITUTE(B30," ",""))</f>
         <v>https://sites.google.com/site/NguyenBaoLan</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="3">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="E31" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenBichThao@gmail.com</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" s="5" t="str">
+      <c r="G31" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenBichThao</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="3">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="E32" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenVanNgoc@gmail.com</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="5" t="str">
+      <c r="G32" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenVanNgoc</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" t="s">
         <v>60</v>
       </c>
-      <c r="I32" s="9"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="3">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D33" s="3" t="str">
+      <c r="E33" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenVanChi@gmail.com</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="5" t="str">
+      <c r="G33" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenVanChi</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="9"/>
+      <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="3">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="E34" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenTuLinh@gmail.com</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G34" s="5" t="str">
+      <c r="G34" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenTuLinh</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" t="s">
         <v>60</v>
       </c>
-      <c r="I34" s="9"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="3">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="E35" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenThuyTrang@gmail.com</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="5" t="str">
+      <c r="G35" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenThuyTrang</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="H35" t="s">
         <v>60</v>
       </c>
-      <c r="I35" s="9"/>
+      <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="3">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="E36" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenTueMan@gmail.com</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G36" s="5" t="str">
+      <c r="G36" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenTueMan</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H36" t="s">
         <v>60</v>
       </c>
-      <c r="I36" s="9"/>
+      <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="3">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="E37" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenThanhTuyet@gmail.com</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G37" s="5" t="str">
+      <c r="G37" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenThanhTuyet</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" t="s">
         <v>40</v>
       </c>
-      <c r="I37" s="9"/>
+      <c r="I37" s="7"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="3">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="E38" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenLeChi@gmail.com</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G38" s="5" t="str">
+      <c r="G38" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenLeChi</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H38" t="s">
         <v>40</v>
       </c>
-      <c r="I38" s="9"/>
+      <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="3">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" t="s">
         <v>112</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D39" s="3" t="str">
+      <c r="E39" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenQuynhThanh@gmail.com</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G39" s="5" t="str">
+      <c r="G39" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenQuynhThanh</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" t="s">
         <v>40</v>
       </c>
-      <c r="I39" s="9"/>
+      <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="3">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>113</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D40" s="3" t="str">
+      <c r="E40" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenMinhTam@gmail.com</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="F40" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G40" s="5" t="str">
+      <c r="G40" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenMinhTam</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="H40" t="s">
         <v>40</v>
       </c>
-      <c r="I40" s="9"/>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="3">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="E41" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenXuyenChi@gmail.com</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G41" s="5" t="str">
+      <c r="G41" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenXuyenChi</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H41" t="s">
         <v>40</v>
       </c>
-      <c r="I41" s="9"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="3">
+      <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="E42" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenXuanLan@gmail.com</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G42" s="5" t="str">
+      <c r="G42" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenXuanLan</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="H42" t="s">
         <v>116</v>
       </c>
-      <c r="I42" s="9"/>
+      <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="3">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="E43" s="1" t="str">
         <f t="shared" si="4"/>
         <v>NguyenPhuongKhanhHuyen@gmail.com</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G43" s="5" t="str">
+      <c r="G43" t="str">
         <f t="shared" si="5"/>
         <v>https://sites.google.com/site/NguyenPhuongKhanhHuyen</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H43" t="s">
         <v>116</v>
       </c>
-      <c r="I43" s="9"/>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="3">
+      <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" t="s">
         <v>119</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="3" t="str">
+      <c r="E44" s="1" t="str">
         <f t="shared" si="4"/>
         <v>VoHaiNam@gmail.com</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G44" s="5" t="str">
+      <c r="G44" t="str">
         <f>CONCATENATE("Http://www.author_","",SUBSTITUTE(B44," ",""),"/wordpress.com")</f>
         <v>Http://www.author_VoHaiNam/wordpress.com</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" t="s">
         <v>116</v>
       </c>
-      <c r="I44" s="9"/>
+      <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="3">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" t="s">
         <v>127</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D45" s="3" t="str">
-        <f t="shared" ref="D45:D58" si="6">CONCATENATE(SUBSTITUTE(B45," ",""),"",,"@gmail.com")</f>
+      <c r="E45" s="1" t="str">
+        <f t="shared" ref="E45:E58" si="6">CONCATENATE(SUBSTITUTE(B45," ",""),"",,"@gmail.com")</f>
         <v>AnSonTung@gmail.com</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G45" s="5" t="str">
+      <c r="G45" t="str">
         <f t="shared" ref="G45:G58" si="7">CONCATENATE("Http://www.author_","",SUBSTITUTE(B45," ",""),"/wordpress.com")</f>
         <v>Http://www.author_AnSonTung/wordpress.com</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H45" t="s">
         <v>116</v>
       </c>
-      <c r="I45" s="9"/>
+      <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="3">
+      <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" t="s">
         <v>128</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="E46" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnCaoTho@gmail.com</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="F46" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G46" s="5" t="str">
+      <c r="G46" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnCaoTho/wordpress.com</v>
       </c>
-      <c r="H46" s="5" t="s">
+      <c r="H46" t="s">
         <v>116</v>
       </c>
-      <c r="I46" s="9"/>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="3">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" t="s">
+        <v>125</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="E47" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnThanhChau@gmail.com</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G47" s="5" t="str">
+      <c r="G47" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnThanhChau/wordpress.com</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="H47" t="s">
         <v>116</v>
       </c>
-      <c r="I47" s="9"/>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="3">
+      <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D48" s="3" t="str">
+      <c r="E48" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnHungÐao@gmail.com</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="F48" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G48" s="5" t="str">
+      <c r="G48" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnHungÐao/wordpress.com</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="H48" t="s">
         <v>116</v>
       </c>
-      <c r="I48" s="9"/>
+      <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="3">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" t="s">
         <v>133</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D49" s="3" t="str">
+      <c r="E49" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnNgocHa@gmail.com</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="F49" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F49" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G49" s="5" t="str">
+      <c r="G49" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnNgocHa/wordpress.com</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H49" t="s">
         <v>60</v>
       </c>
-      <c r="I49" s="9"/>
+      <c r="I49" s="7"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="3">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" t="s">
         <v>135</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D50" s="3" t="str">
+      <c r="E50" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnThienTrang@gmail.com</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="F50" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G50" s="5" t="str">
+      <c r="G50" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnThienTrang/wordpress.com</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="H50" t="s">
         <v>60</v>
       </c>
-      <c r="I50" s="9"/>
+      <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="3">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" t="s">
         <v>136</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D51" s="3" t="str">
+      <c r="E51" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnAnhNgoc@gmail.com</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="F51" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F51" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G51" s="5" t="str">
+      <c r="G51" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnAnhNgoc/wordpress.com</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" t="s">
         <v>60</v>
       </c>
-      <c r="I51" s="9"/>
+      <c r="I51" s="7"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="3">
+      <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D52" s="3" t="str">
+      <c r="E52" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnBichHao@gmail.com</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="F52" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="5" t="str">
+      <c r="G52" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnBichHao/wordpress.com</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H52" t="s">
         <v>60</v>
       </c>
-      <c r="I52" s="9"/>
+      <c r="I52" s="7"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="3">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D53" s="3" t="str">
+      <c r="E53" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnManNhi@gmail.com</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="F53" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="5" t="str">
+      <c r="G53" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnManNhi/wordpress.com</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H53" t="s">
         <v>60</v>
       </c>
-      <c r="I53" s="9"/>
+      <c r="I53" s="7"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="3">
+      <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D54" s="3" t="str">
+      <c r="E54" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnThaiThanh@gmail.com</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="F54" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G54" s="5" t="str">
+      <c r="G54" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnThaiThanh/wordpress.com</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" t="s">
         <v>140</v>
       </c>
-      <c r="I54" s="9"/>
+      <c r="I54" s="7"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="3">
+      <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" t="s">
         <v>141</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D55" s="3" t="str">
+      <c r="E55" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnBaoHa@gmail.com</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="F55" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F55" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" s="5" t="str">
+      <c r="G55" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnBaoHa/wordpress.com</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H55" t="s">
         <v>143</v>
       </c>
-      <c r="I55" s="9"/>
+      <c r="I55" s="7"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="3">
+      <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D56" s="3" t="str">
+      <c r="E56" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnNgocQuynh@gmail.com</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="F56" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F56" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G56" s="5" t="str">
+      <c r="G56" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnNgocQuynh/wordpress.com</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H56" t="s">
         <v>146</v>
       </c>
-      <c r="I56" s="9"/>
+      <c r="I56" s="7"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="3">
+      <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D57" s="3" t="str">
+      <c r="E57" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnPhuongBaoHan@gmail.com</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="F57" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G57" s="5" t="str">
+      <c r="G57" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnPhuongBaoHan/wordpress.com</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H57" t="s">
         <v>143</v>
       </c>
-      <c r="I57" s="9"/>
+      <c r="I57" s="7"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="3">
+      <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" t="s">
         <v>148</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D58" s="3" t="str">
+      <c r="E58" s="1" t="str">
         <f t="shared" si="6"/>
         <v>AnHaiYen@gmail.com</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="F58" t="s">
         <v>65</v>
       </c>
-      <c r="F58" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="G58" s="5" t="str">
+      <c r="G58" t="str">
         <f t="shared" si="7"/>
         <v>Http://www.author_AnHaiYen/wordpress.com</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H58" t="s">
         <v>150</v>
       </c>
-      <c r="I58" s="9"/>
+      <c r="I58" s="7"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="3"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="9"/>
+      <c r="D59" s="4"/>
+      <c r="I59" s="7"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="3"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="9"/>
+      <c r="D60" s="4"/>
+      <c r="I60" s="7"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="3"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="9"/>
+      <c r="D61" s="4"/>
+      <c r="I61" s="7"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="3"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="9"/>
+      <c r="D62" s="4"/>
+      <c r="I62" s="7"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="3"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="9"/>
+      <c r="D63" s="4"/>
+      <c r="I63" s="7"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="3"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="9"/>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="3"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="9"/>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="3"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="9"/>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="3"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="9"/>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="3"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="9"/>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="3"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="9"/>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="3"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="9"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="3"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="9"/>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="3"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="9"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="3"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="9"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="3"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="10"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="9"/>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="3"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="9"/>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="3"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="9"/>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="3"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="9"/>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="3"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="9"/>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="3"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="9"/>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="3"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="9"/>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="3"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="9"/>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="3"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="9"/>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="3"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="6"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="9"/>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="3"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="9"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="3"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="9"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="3"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="9"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="3"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="9"/>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="3"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="9"/>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="3"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="9"/>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="3"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="6"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="9"/>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="3"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="6"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
-      <c r="I91" s="9"/>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="3"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="9"/>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="3"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="9"/>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="3"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="9"/>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95" s="3"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="9"/>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="3"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="5"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="9"/>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="3"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="9"/>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="3"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="6"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="9"/>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99" s="3"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="9"/>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="3"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="9"/>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" s="3"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="10"/>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="9"/>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" s="3"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="10"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="9"/>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="3"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="10"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="5"/>
-      <c r="I103" s="9"/>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="3"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="10"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="9"/>
-    </row>
-    <row r="105" spans="1:9">
-      <c r="A105" s="3"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="10"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-      <c r="I105" s="9"/>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="A106" s="3"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="10"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-      <c r="I106" s="9"/>
-    </row>
-    <row r="107" spans="1:9">
-      <c r="A107" s="3"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="6"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="10"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="5"/>
-      <c r="I107" s="9"/>
-    </row>
-    <row r="108" spans="1:9">
-      <c r="A108" s="3"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="10"/>
-      <c r="G108" s="5"/>
-      <c r="H108" s="5"/>
-      <c r="I108" s="9"/>
-    </row>
-    <row r="109" spans="1:9">
-      <c r="A109" s="3"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="6"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="10"/>
-      <c r="G109" s="5"/>
-      <c r="H109" s="5"/>
-      <c r="I109" s="9"/>
-    </row>
-    <row r="110" spans="1:9">
-      <c r="A110" s="3"/>
-      <c r="B110" s="5"/>
-      <c r="C110" s="6"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="10"/>
-      <c r="G110" s="5"/>
-      <c r="H110" s="5"/>
-      <c r="I110" s="9"/>
-    </row>
-    <row r="111" spans="1:9">
-      <c r="A111" s="3"/>
-      <c r="B111" s="5"/>
-      <c r="C111" s="6"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="10"/>
-      <c r="G111" s="5"/>
-      <c r="H111" s="5"/>
-      <c r="I111" s="9"/>
-    </row>
-    <row r="112" spans="1:9">
-      <c r="A112" s="3"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="6"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="10"/>
-      <c r="G112" s="5"/>
-      <c r="H112" s="5"/>
-      <c r="I112" s="9"/>
-    </row>
-    <row r="113" spans="1:9">
-      <c r="A113" s="3"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="6"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="10"/>
-      <c r="G113" s="5"/>
-      <c r="H113" s="5"/>
-      <c r="I113" s="9"/>
-    </row>
-    <row r="114" spans="1:9">
-      <c r="A114" s="3"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="6"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="10"/>
-      <c r="G114" s="5"/>
-      <c r="H114" s="5"/>
-      <c r="I114" s="9"/>
-    </row>
-    <row r="115" spans="1:9">
-      <c r="A115" s="3"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="6"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="10"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="5"/>
-      <c r="I115" s="9"/>
-    </row>
-    <row r="116" spans="1:9">
-      <c r="A116" s="3"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="6"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="10"/>
-      <c r="G116" s="5"/>
-      <c r="H116" s="5"/>
-      <c r="I116" s="9"/>
-    </row>
-    <row r="117" spans="1:9">
-      <c r="A117" s="3"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="6"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="10"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="5"/>
-      <c r="I117" s="9"/>
-    </row>
-    <row r="118" spans="1:9">
-      <c r="A118" s="3"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="6"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="10"/>
-      <c r="G118" s="5"/>
-      <c r="H118" s="5"/>
-      <c r="I118" s="9"/>
-    </row>
-    <row r="119" spans="1:9">
-      <c r="A119" s="3"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="10"/>
-      <c r="G119" s="5"/>
-      <c r="H119" s="5"/>
-      <c r="I119" s="9"/>
-    </row>
-    <row r="120" spans="1:9">
-      <c r="A120" s="3"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="6"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="10"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="5"/>
-      <c r="I120" s="9"/>
+      <c r="D64" s="4"/>
+      <c r="I64" s="7"/>
+    </row>
+    <row r="65" spans="4:9">
+      <c r="D65" s="4"/>
+      <c r="I65" s="7"/>
+    </row>
+    <row r="66" spans="4:9">
+      <c r="D66" s="4"/>
+      <c r="I66" s="7"/>
+    </row>
+    <row r="67" spans="4:9">
+      <c r="D67" s="4"/>
+      <c r="I67" s="7"/>
+    </row>
+    <row r="68" spans="4:9">
+      <c r="D68" s="4"/>
+      <c r="I68" s="7"/>
+    </row>
+    <row r="69" spans="4:9">
+      <c r="D69" s="4"/>
+      <c r="I69" s="7"/>
+    </row>
+    <row r="70" spans="4:9">
+      <c r="D70" s="4"/>
+      <c r="I70" s="7"/>
+    </row>
+    <row r="71" spans="4:9">
+      <c r="D71" s="4"/>
+      <c r="I71" s="7"/>
+    </row>
+    <row r="72" spans="4:9">
+      <c r="D72" s="4"/>
+      <c r="I72" s="7"/>
+    </row>
+    <row r="73" spans="4:9">
+      <c r="D73" s="4"/>
+      <c r="I73" s="7"/>
+    </row>
+    <row r="74" spans="4:9">
+      <c r="D74" s="4"/>
+      <c r="I74" s="7"/>
+    </row>
+    <row r="75" spans="4:9">
+      <c r="D75" s="4"/>
+      <c r="I75" s="7"/>
+    </row>
+    <row r="76" spans="4:9">
+      <c r="D76" s="4"/>
+      <c r="I76" s="7"/>
+    </row>
+    <row r="77" spans="4:9">
+      <c r="D77" s="4"/>
+      <c r="I77" s="7"/>
+    </row>
+    <row r="78" spans="4:9">
+      <c r="D78" s="4"/>
+      <c r="I78" s="7"/>
+    </row>
+    <row r="79" spans="4:9">
+      <c r="D79" s="4"/>
+      <c r="I79" s="7"/>
+    </row>
+    <row r="80" spans="4:9">
+      <c r="D80" s="4"/>
+      <c r="I80" s="7"/>
+    </row>
+    <row r="81" spans="4:9">
+      <c r="D81" s="4"/>
+      <c r="I81" s="7"/>
+    </row>
+    <row r="82" spans="4:9">
+      <c r="D82" s="4"/>
+      <c r="I82" s="7"/>
+    </row>
+    <row r="83" spans="4:9">
+      <c r="D83" s="4"/>
+      <c r="I83" s="7"/>
+    </row>
+    <row r="84" spans="4:9">
+      <c r="D84" s="4"/>
+      <c r="I84" s="7"/>
+    </row>
+    <row r="85" spans="4:9">
+      <c r="D85" s="4"/>
+      <c r="I85" s="7"/>
+    </row>
+    <row r="86" spans="4:9">
+      <c r="D86" s="4"/>
+      <c r="I86" s="7"/>
+    </row>
+    <row r="87" spans="4:9">
+      <c r="D87" s="4"/>
+      <c r="I87" s="7"/>
+    </row>
+    <row r="88" spans="4:9">
+      <c r="D88" s="4"/>
+      <c r="I88" s="7"/>
+    </row>
+    <row r="89" spans="4:9">
+      <c r="D89" s="4"/>
+      <c r="I89" s="7"/>
+    </row>
+    <row r="90" spans="4:9">
+      <c r="D90" s="4"/>
+      <c r="I90" s="7"/>
+    </row>
+    <row r="91" spans="4:9">
+      <c r="D91" s="4"/>
+      <c r="I91" s="7"/>
+    </row>
+    <row r="92" spans="4:9">
+      <c r="D92" s="4"/>
+      <c r="I92" s="7"/>
+    </row>
+    <row r="93" spans="4:9">
+      <c r="D93" s="4"/>
+      <c r="I93" s="7"/>
+    </row>
+    <row r="94" spans="4:9">
+      <c r="D94" s="4"/>
+      <c r="I94" s="7"/>
+    </row>
+    <row r="95" spans="4:9">
+      <c r="D95" s="4"/>
+      <c r="I95" s="7"/>
+    </row>
+    <row r="96" spans="4:9">
+      <c r="D96" s="4"/>
+      <c r="I96" s="7"/>
+    </row>
+    <row r="97" spans="4:9">
+      <c r="D97" s="4"/>
+      <c r="I97" s="7"/>
+    </row>
+    <row r="98" spans="4:9">
+      <c r="D98" s="4"/>
+      <c r="I98" s="7"/>
+    </row>
+    <row r="99" spans="4:9">
+      <c r="D99" s="4"/>
+      <c r="I99" s="7"/>
+    </row>
+    <row r="100" spans="4:9">
+      <c r="D100" s="4"/>
+      <c r="I100" s="7"/>
+    </row>
+    <row r="101" spans="4:9">
+      <c r="D101" s="4"/>
+      <c r="I101" s="7"/>
+    </row>
+    <row r="102" spans="4:9">
+      <c r="D102" s="4"/>
+      <c r="I102" s="7"/>
+    </row>
+    <row r="103" spans="4:9">
+      <c r="D103" s="4"/>
+      <c r="I103" s="7"/>
+    </row>
+    <row r="104" spans="4:9">
+      <c r="D104" s="4"/>
+      <c r="I104" s="7"/>
+    </row>
+    <row r="105" spans="4:9">
+      <c r="D105" s="4"/>
+      <c r="I105" s="7"/>
+    </row>
+    <row r="106" spans="4:9">
+      <c r="D106" s="4"/>
+      <c r="I106" s="7"/>
+    </row>
+    <row r="107" spans="4:9">
+      <c r="D107" s="4"/>
+      <c r="I107" s="7"/>
+    </row>
+    <row r="108" spans="4:9">
+      <c r="D108" s="4"/>
+      <c r="I108" s="7"/>
+    </row>
+    <row r="109" spans="4:9">
+      <c r="D109" s="4"/>
+      <c r="I109" s="7"/>
+    </row>
+    <row r="110" spans="4:9">
+      <c r="D110" s="4"/>
+      <c r="I110" s="7"/>
+    </row>
+    <row r="111" spans="4:9">
+      <c r="D111" s="4"/>
+      <c r="I111" s="7"/>
+    </row>
+    <row r="112" spans="4:9">
+      <c r="D112" s="4"/>
+      <c r="I112" s="7"/>
+    </row>
+    <row r="113" spans="4:9">
+      <c r="D113" s="4"/>
+      <c r="I113" s="7"/>
+    </row>
+    <row r="114" spans="4:9">
+      <c r="D114" s="4"/>
+      <c r="I114" s="7"/>
+    </row>
+    <row r="115" spans="4:9">
+      <c r="D115" s="4"/>
+      <c r="I115" s="7"/>
+    </row>
+    <row r="116" spans="4:9">
+      <c r="D116" s="4"/>
+      <c r="I116" s="7"/>
+    </row>
+    <row r="117" spans="4:9">
+      <c r="D117" s="4"/>
+      <c r="I117" s="7"/>
+    </row>
+    <row r="118" spans="4:9">
+      <c r="D118" s="4"/>
+      <c r="I118" s="7"/>
+    </row>
+    <row r="119" spans="4:9">
+      <c r="D119" s="4"/>
+      <c r="I119" s="7"/>
+    </row>
+    <row r="120" spans="4:9">
+      <c r="D120" s="4"/>
+      <c r="I120" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>